<commit_message>
Updated runsheet for second pilot
</commit_message>
<xml_diff>
--- a/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
+++ b/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allison\soc_xsit\soc_xsit_expts\soc_xsit_ipad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15024" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>subid</t>
   </si>
@@ -46,6 +51,24 @@
   </si>
   <si>
     <t>SOC_XSIT_1</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_2</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_3</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_4</t>
   </si>
 </sst>
 </file>
@@ -249,6 +272,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -577,12 +608,12 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,298 +639,371 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B2" s="2">
+        <v>41849</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40079</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>4.8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>41849</v>
+      </c>
+      <c r="C3" s="2">
+        <v>40618</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>3.3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <v>41849</v>
+      </c>
+      <c r="C4" s="2">
+        <v>39775</v>
+      </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>5.6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>41849</v>
+      </c>
+      <c r="C5" s="2">
+        <v>40108</v>
+      </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>4.7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="12.75" customHeight="1">
+    <row r="17" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="12.75" customHeight="1">
+    <row r="18" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="12.75" customHeight="1">
+    <row r="19" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="12.75" customHeight="1">
+    <row r="20" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="12.75" customHeight="1">
+    <row r="21" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="12.75" customHeight="1">
+    <row r="22" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="12.75" customHeight="1">
+    <row r="23" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="12.75" customHeight="1">
+    <row r="24" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="12.75" customHeight="1">
+    <row r="25" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="12.75" customHeight="1">
+    <row r="26" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="12.75" customHeight="1">
+    <row r="27" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="12.75" customHeight="1">
+    <row r="28" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="12.75" customHeight="1">
+    <row r="29" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="12.75" customHeight="1">
+    <row r="30" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="12.75" customHeight="1">
+    <row r="31" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="12.75" customHeight="1">
+    <row r="32" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="2:4" ht="12.75" customHeight="1">
+    <row r="33" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="2:4" ht="12.75" customHeight="1">
+    <row r="34" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="2:4" ht="12.75" customHeight="1">
+    <row r="35" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="2:4" ht="12.75" customHeight="1">
+    <row r="36" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="2:4" ht="12.75" customHeight="1">
+    <row r="37" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="2:4" ht="12.75" customHeight="1">
+    <row r="38" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="2:4" ht="12.75" customHeight="1">
+    <row r="39" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="2:4" ht="12.75" customHeight="1">
+    <row r="40" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="2:4" ht="12.75" customHeight="1">
+    <row r="41" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="2:4" ht="12.75" customHeight="1">
+    <row r="42" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="2:4" ht="12.75" customHeight="1">
+    <row r="43" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="2:4" ht="12.75" customHeight="1">
+    <row r="44" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="2:4" ht="12.75" customHeight="1">
+    <row r="45" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="2:4" ht="12.75" customHeight="1">
+    <row r="46" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="2:4" ht="12.75" customHeight="1">
+    <row r="47" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="2:4" ht="12.75" customHeight="1">
+    <row r="48" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="2:4" ht="12.75" customHeight="1">
+    <row r="49" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="2:4" ht="12.75" customHeight="1">
+    <row r="50" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="2:4" ht="12.75" customHeight="1">
+    <row r="51" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="2:4" ht="12.75" customHeight="1">
+    <row r="52" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="2:4" ht="12.75" customHeight="1">
+    <row r="53" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="2:4" ht="12.75" customHeight="1">
+    <row r="54" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="2:4" ht="12.75" customHeight="1">
+    <row r="55" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="2:4" ht="12.75" customHeight="1">
+    <row r="56" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="2:4" ht="12.75" customHeight="1">
+    <row r="57" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="2:4" ht="12.75" customHeight="1">
+    <row r="58" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="2:4" ht="12.75" customHeight="1">
+    <row r="59" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="2:4" ht="12.75" customHeight="1">
+    <row r="60" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="4"/>

</xml_diff>

<commit_message>
Ipad runsheet updated through 17
</commit_message>
<xml_diff>
--- a/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
+++ b/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>subid</t>
   </si>
@@ -69,6 +69,45 @@
   </si>
   <si>
     <t>SOC_XSIT_4</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_5</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_6</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_7</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_8</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_9</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_10</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_11</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_12</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_13</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_14</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_15</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_16</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_17</t>
   </si>
 </sst>
 </file>
@@ -608,7 +647,7 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -734,136 +773,347 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C6" s="2">
+        <v>39957</v>
+      </c>
       <c r="D6" s="1"/>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C7" s="2">
+        <v>39968</v>
+      </c>
       <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C8" s="2">
+        <v>40147</v>
+      </c>
       <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C9" s="2">
+        <v>40372</v>
+      </c>
       <c r="D9" s="1"/>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>3.11</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C10" s="2">
+        <v>40315</v>
+      </c>
       <c r="D10" s="1"/>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C11" s="2">
+        <v>40386</v>
+      </c>
       <c r="D11" s="1"/>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2">
+        <v>41851</v>
+      </c>
+      <c r="C12" s="2">
+        <v>40289</v>
+      </c>
       <c r="D12" s="1"/>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>4.2</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2">
+        <v>41852</v>
+      </c>
+      <c r="C13" s="2">
+        <v>40339</v>
+      </c>
       <c r="D13" s="1"/>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <v>41852</v>
+      </c>
+      <c r="C14" s="2">
+        <v>40304</v>
+      </c>
       <c r="D14" s="1"/>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>41852</v>
+      </c>
+      <c r="C15" s="2">
+        <v>39995</v>
+      </c>
       <c r="D15" s="1"/>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2">
+        <v>41852</v>
+      </c>
+      <c r="C16" s="2">
+        <v>39948</v>
+      </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2">
+        <v>41852</v>
+      </c>
+      <c r="C17" s="2">
+        <v>39971</v>
+      </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2">
+        <v>41855</v>
+      </c>
+      <c r="C18" s="2">
+        <v>40421</v>
+      </c>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>3.9</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="1"/>

</xml_diff>

<commit_message>
Updated csv for ipad as of 8/6
</commit_message>
<xml_diff>
--- a/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
+++ b/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
@@ -647,7 +647,7 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Between subjects this/one finished
</commit_message>
<xml_diff>
--- a/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
+++ b/soc_xsit_expts/soc_xsit_ipad/SOC_XSIT_Runsheet_Bing.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>subid</t>
   </si>
@@ -108,6 +108,36 @@
   </si>
   <si>
     <t>SOC_XSIT_17</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_18</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_19</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_20</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_21</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_22</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_23</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_24</t>
+  </si>
+  <si>
+    <t>SOC_XSIT_25</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -647,7 +677,7 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1049,44 +1079,108 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <v>41856</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2">
+        <v>41856</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2">
+        <v>41856</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2">
+        <v>41856</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="2">
+        <v>41856</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2">
+        <v>41857</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="2">
+        <v>41857</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="2">
+        <v>41858</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>

</xml_diff>